<commit_message>
Add new icons and fix API endpoint
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zane2\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Typescript\fake-trap\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46989D9-0581-4451-B566-12C22A5D6142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B286BC42-A7BC-4EC8-A76C-567C737F05AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="4815" windowWidth="21600" windowHeight="11295" xr2:uid="{68A8FC0D-FC19-4E22-94B1-584C5F3416C9}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{68A8FC0D-FC19-4E22-94B1-584C5F3416C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>id_quiz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>question_text</t>
   </si>
@@ -435,14 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0770BC4-CBF8-4A39-94AC-28F080E6C18A}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
@@ -450,12 +448,12 @@
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -466,27 +464,21 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>